<commit_message>
added login_helper for code reusability.
</commit_message>
<xml_diff>
--- a/fund_transfers.xlsx
+++ b/fund_transfers.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1433,6 +1433,1156 @@
         <v>2781</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:13</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>5078</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:16</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:20</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>8477</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:24</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:27</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>7698</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:31</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>2339</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:35</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>9581</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:38</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>9874</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:42</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:45</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:49</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>2648</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:53</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:30:56</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>8799</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:31:00</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:31:04</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:38</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>8503</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:42</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>7744</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:45</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>7388</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:49</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>7690</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:53</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>9189</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:36:56</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:00</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:04</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>9498</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:07</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>6539</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:11</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:15</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:18</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>5299</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:22</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>6327</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:25</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>3293</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:29</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:33</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>6090</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:36</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:40</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>6387</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:44</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:47</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:51</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:54</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>7416</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:37:58</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:02</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:05</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>9606</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:09</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>9401</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:13</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:16</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:20</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>8473</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:24</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:27</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:31</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>7497</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:34</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:38</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>8536</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:42</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>4126</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:45</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>9741</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:49</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:53</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:38:56</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>5569</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:00</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:04</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>3785</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:07</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:11</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>7762</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:14</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>5898</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:18</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>3503</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:22</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>9516</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:25</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:29</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:33</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>7810</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:36</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>6606</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:40</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:44</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>5277</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:47</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:51</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>5855</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:55</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>7127</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:39:58</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>7679</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:02</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:05</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:09</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>6267</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:13</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>9458</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:16</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>8112</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:20</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>9246</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:24</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>9552</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:27</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>9411</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:31</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>5089</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:35</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>9866</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:38</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:42</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>9778</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:46</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>5113</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:49</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:53</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>2064</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:40:57</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>3487</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:00</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>3224</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:04</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>5423</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:08</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>8311</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:11</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>9182</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:15</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:18</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:22</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:26</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:29</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:33</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>6076</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:37</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>6786</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:40</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>2604</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:44</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:48</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>7202</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:51</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>8341</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:55</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>8893</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:41:59</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:02</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:06</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>2683</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:10</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>6540</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:13</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:17</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:21</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>4485</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:24</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:28</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>7454</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:32</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:35</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>3466</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2025-10-05 18:42:39</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>5612</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>